<commit_message>
Complete Practical 3 & 4
</commit_message>
<xml_diff>
--- a/Practical Files/exels/Practical-3.xlsx
+++ b/Practical Files/exels/Practical-3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vatsal\Desktop\Sem4\DAA\Practical Files\exels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Sem4\DAA\Practical Files\exels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA88E52-3CE3-4544-A253-7DDA7AF6BC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404FD299-64C0-4C5F-AF2A-A66008A5159E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15336" yWindow="684" windowWidth="15336" windowHeight="16548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Bubble Sort</t>
   </si>
@@ -47,18 +47,36 @@
   <si>
     <t>Number of Inputs</t>
   </si>
+  <si>
+    <t xml:space="preserve">Random Quick Sort </t>
+  </si>
+  <si>
+    <t>Random Quick Sort</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -69,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -77,12 +95,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -134,14 +223,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Sorting</a:t>
+              <a:rPr lang="en-IN"/>
+              <a:t>Sorting Methods</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Methods (Random Data)</a:t>
+              <a:rPr lang="en-IN" baseline="0"/>
+              <a:t> (Random Data)</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-IN"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -177,25 +266,25 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Bubble Sort</c:v>
+                  <c:v>Number of Inputs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -218,12 +307,12 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -236,46 +325,13 @@
                 <c:pt idx="3">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>435</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>780</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1225</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7655-42DB-95E9-7A875A220BCC}"/>
+              <c16:uniqueId val="{00000000-F5EA-400E-A496-A7AD288B3BE3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -284,17 +340,17 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Insertion Sort</c:v>
+                  <c:v>Bubble Sort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -317,64 +373,31 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>104</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>263</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>474</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>605</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7655-42DB-95E9-7A875A220BCC}"/>
+              <c16:uniqueId val="{00000001-F5EA-400E-A496-A7AD288B3BE3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -383,17 +406,17 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Selection Sort</c:v>
+                  <c:v>Insertion Sort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -416,64 +439,31 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>409</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$2:$D$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>435</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>780</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1225</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-7655-42DB-95E9-7A875A220BCC}"/>
+              <c16:uniqueId val="{00000002-F5EA-400E-A496-A7AD288B3BE3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -482,17 +472,17 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Quick Sort</c:v>
+                  <c:v>Selection Sort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -515,64 +505,31 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$2:$E$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>164</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>228</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-7655-42DB-95E9-7A875A220BCC}"/>
+              <c16:uniqueId val="{00000003-F5EA-400E-A496-A7AD288B3BE3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -581,17 +538,17 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>Sheet1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Merge Sort</c:v>
+                  <c:v>Quick Sort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
@@ -614,64 +571,169 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$E$2:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F5EA-400E-A496-A7AD288B3BE3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random Quick Sort </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$7</c:f>
+              <c:f>Sheet1!$F$2:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>176</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>296</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>432</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>572</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-7655-42DB-95E9-7A875A220BCC}"/>
+              <c16:uniqueId val="{00000005-F5EA-400E-A496-A7AD288B3BE3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Merge Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>109</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-F5EA-400E-A496-A7AD288B3BE3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -683,30 +745,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="193823647"/>
-        <c:axId val="193824479"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="193823647"/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="973440288"/>
+        <c:axId val="973445280"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="973440288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -716,8 +766,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -744,12 +794,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="193824479"/>
+        <c:crossAx val="973445280"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="193824479"/>
+        <c:axId val="973445280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,14 +828,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -806,9 +853,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="193823647"/>
+        <c:crossAx val="973440288"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -851,13 +898,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -927,12 +967,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Sorting Methods (Sorted Data)</a:t>
+              <a:rPr lang="en-IN"/>
+              <a:t>Sorting</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:r>
+              <a:rPr lang="en-IN" baseline="0"/>
+              <a:t> Methods (Sorted Data)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -968,25 +1010,25 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>Sheet1!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Bubble Sort</c:v>
+                  <c:v>Number of Inputs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1009,9 +1051,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$7</c:f>
+              <c:f>Sheet1!$A$13:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1035,38 +1077,11 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$I$2:$I$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>435</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>780</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1225</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
+          </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F489-473B-9354-B5F038F5FA31}"/>
+              <c16:uniqueId val="{00000000-DFEA-48B3-A6A2-A7A93A5A367F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1075,17 +1090,17 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$1</c:f>
+              <c:f>Sheet1!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Insertion Sort</c:v>
+                  <c:v>Bubble Sort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -1108,64 +1123,37 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$7</c:f>
+              <c:f>Sheet1!$B$13:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>435</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>780</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>1225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$J$2:$J$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>49</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
+          </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F489-473B-9354-B5F038F5FA31}"/>
+              <c16:uniqueId val="{00000001-DFEA-48B3-A6A2-A7A93A5A367F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1174,17 +1162,17 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$1</c:f>
+              <c:f>Sheet1!$C$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Selection Sort</c:v>
+                  <c:v>Insertion Sort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -1207,64 +1195,37 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$7</c:f>
+              <c:f>Sheet1!$C$13:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$K$2:$K$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>435</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>780</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1225</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
+          </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F489-473B-9354-B5F038F5FA31}"/>
+              <c16:uniqueId val="{00000002-DFEA-48B3-A6A2-A7A93A5A367F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1273,17 +1234,17 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$1</c:f>
+              <c:f>Sheet1!$D$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Quick Sort</c:v>
+                  <c:v>Selection Sort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -1306,36 +1267,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$L$2:$L$7</c:f>
+              <c:f>Sheet1!$D$13:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1359,11 +1293,11 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
+          </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-F489-473B-9354-B5F038F5FA31}"/>
+              <c16:uniqueId val="{00000003-DFEA-48B3-A6A2-A7A93A5A367F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1372,17 +1306,17 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$1</c:f>
+              <c:f>Sheet1!$E$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Merge Sort</c:v>
+                  <c:v>Quick Sort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
@@ -1405,64 +1339,187 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$7</c:f>
+              <c:f>Sheet1!$E$13:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>435</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>780</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>1225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-DFEA-48B3-A6A2-A7A93A5A367F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random Quick Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$7</c:f>
+              <c:f>Sheet1!$F$13:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>68</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>176</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>296</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>432</c:v>
+                  <c:v>257</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>572</c:v>
+                  <c:v>235</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
+          </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-F489-473B-9354-B5F038F5FA31}"/>
+              <c16:uniqueId val="{00000005-DFEA-48B3-A6A2-A7A93A5A367F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Merge Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$13:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>153</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-DFEA-48B3-A6A2-A7A93A5A367F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1474,30 +1531,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="363427343"/>
-        <c:axId val="363425679"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="363427343"/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="973464416"/>
+        <c:axId val="973460256"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="973464416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1507,8 +1552,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1535,12 +1580,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363425679"/>
+        <c:crossAx val="973460256"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="363425679"/>
+        <c:axId val="973460256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1566,14 +1614,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1597,9 +1639,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363427343"/>
+        <c:crossAx val="973464416"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1758,7 +1800,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1785,8 +1827,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1887,7 +1929,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1919,10 +1961,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1962,23 +2004,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2083,8 +2124,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2216,20 +2257,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2243,17 +2283,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2274,7 +2303,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2301,8 +2330,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2403,7 +2432,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2435,10 +2464,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2478,23 +2507,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2599,8 +2627,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2732,20 +2760,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2759,17 +2786,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2793,23 +2809,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>733599</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>22168</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>598715</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>251650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>278131</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>22168</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>310564</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>42901</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A49B4DA8-716D-4A71-8612-22220DBF83D6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68870A85-C5E2-4646-9938-D5282E5B52F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2830,22 +2846,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>117817</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>32239</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>84364</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>422617</xdr:colOff>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>32239</xdr:rowOff>
+      <xdr:rowOff>119743</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B69E27E-6516-47B0-9B11-207B481780A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEBE043C-7484-4224-B7A5-050BD40E7D67}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3129,430 +3145,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="B2" s="4">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8</v>
+      </c>
+      <c r="G2" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4">
+        <v>45</v>
+      </c>
+      <c r="C3" s="4">
+        <v>27</v>
+      </c>
+      <c r="D3" s="4">
+        <v>45</v>
+      </c>
+      <c r="E3" s="4">
+        <v>20</v>
+      </c>
+      <c r="F3" s="4">
+        <v>34</v>
+      </c>
+      <c r="G3" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4">
+        <v>190</v>
+      </c>
+      <c r="C4" s="4">
+        <v>108</v>
+      </c>
+      <c r="D4" s="4">
+        <v>190</v>
+      </c>
+      <c r="E4" s="4">
+        <v>67</v>
+      </c>
+      <c r="F4" s="4">
+        <v>55</v>
+      </c>
+      <c r="G4" s="4">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>30</v>
+      </c>
+      <c r="B5" s="4">
+        <v>435</v>
+      </c>
+      <c r="C5" s="4">
+        <v>409</v>
+      </c>
+      <c r="D5" s="4">
+        <v>435</v>
+      </c>
+      <c r="E5" s="4">
+        <v>110</v>
+      </c>
+      <c r="F5" s="4">
+        <v>104</v>
+      </c>
+      <c r="G5" s="4">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J1" t="s">
+      <c r="C12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K1" t="s">
+      <c r="D12" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="E12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M1" t="s">
+      <c r="F12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="13" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B13" s="4">
         <v>10</v>
       </c>
-      <c r="C2">
-        <v>11</v>
-      </c>
-      <c r="D2">
+      <c r="C13" s="4">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="E13" s="4">
         <v>10</v>
       </c>
-      <c r="F2">
+      <c r="F13" s="4">
+        <v>7</v>
+      </c>
+      <c r="G13" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4">
+        <v>45</v>
+      </c>
+      <c r="C14" s="4">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4">
+        <v>45</v>
+      </c>
+      <c r="E14" s="4">
+        <v>45</v>
+      </c>
+      <c r="F14" s="4">
         <v>24</v>
       </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>10</v>
-      </c>
-      <c r="J2">
-        <v>4</v>
-      </c>
-      <c r="K2">
-        <v>10</v>
-      </c>
-      <c r="L2">
-        <v>10</v>
-      </c>
-      <c r="M2">
-        <v>24</v>
+      <c r="G14" s="4">
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>45</v>
-      </c>
-      <c r="C3">
-        <v>32</v>
-      </c>
-      <c r="D3">
-        <v>45</v>
-      </c>
-      <c r="E3">
+    <row r="15" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
         <v>20</v>
       </c>
-      <c r="F3">
-        <v>68</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3">
-        <v>45</v>
-      </c>
-      <c r="J3">
-        <v>9</v>
-      </c>
-      <c r="K3">
-        <v>45</v>
-      </c>
-      <c r="L3">
-        <v>45</v>
-      </c>
-      <c r="M3">
-        <v>68</v>
+      <c r="B15" s="4">
+        <v>190</v>
+      </c>
+      <c r="C15" s="4">
+        <v>19</v>
+      </c>
+      <c r="D15" s="4">
+        <v>190</v>
+      </c>
+      <c r="E15" s="4">
+        <v>190</v>
+      </c>
+      <c r="F15" s="4">
+        <v>91</v>
+      </c>
+      <c r="G15" s="4">
+        <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>190</v>
-      </c>
-      <c r="C4">
-        <v>104</v>
-      </c>
-      <c r="D4">
-        <v>190</v>
-      </c>
-      <c r="E4">
-        <v>67</v>
-      </c>
-      <c r="F4">
-        <v>176</v>
-      </c>
-      <c r="H4">
-        <v>20</v>
-      </c>
-      <c r="I4">
-        <v>190</v>
-      </c>
-      <c r="J4">
-        <v>19</v>
-      </c>
-      <c r="K4">
-        <v>190</v>
-      </c>
-      <c r="L4">
-        <v>190</v>
-      </c>
-      <c r="M4">
-        <v>176</v>
+    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>30</v>
+      </c>
+      <c r="B16" s="4">
+        <v>435</v>
+      </c>
+      <c r="C16" s="4">
+        <v>29</v>
+      </c>
+      <c r="D16" s="4">
+        <v>435</v>
+      </c>
+      <c r="E16" s="4">
+        <v>435</v>
+      </c>
+      <c r="F16" s="4">
+        <v>139</v>
+      </c>
+      <c r="G16" s="4">
+        <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>30</v>
-      </c>
-      <c r="B5">
-        <v>435</v>
-      </c>
-      <c r="C5">
-        <v>263</v>
-      </c>
-      <c r="D5">
-        <v>435</v>
-      </c>
-      <c r="E5">
-        <v>110</v>
-      </c>
-      <c r="F5">
-        <v>296</v>
-      </c>
-      <c r="H5">
-        <v>30</v>
-      </c>
-      <c r="I5">
-        <v>435</v>
-      </c>
-      <c r="J5">
-        <v>29</v>
-      </c>
-      <c r="K5">
-        <v>435</v>
-      </c>
-      <c r="L5">
-        <v>435</v>
-      </c>
-      <c r="M5">
-        <v>296</v>
+    <row r="17" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>40</v>
+      </c>
+      <c r="B17" s="4">
+        <v>780</v>
+      </c>
+      <c r="C17" s="4">
+        <v>39</v>
+      </c>
+      <c r="D17" s="4">
+        <v>780</v>
+      </c>
+      <c r="E17" s="4">
+        <v>780</v>
+      </c>
+      <c r="F17" s="4">
+        <v>257</v>
+      </c>
+      <c r="G17" s="4">
+        <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>40</v>
-      </c>
-      <c r="B6">
-        <v>780</v>
-      </c>
-      <c r="C6">
-        <v>474</v>
-      </c>
-      <c r="D6">
-        <v>780</v>
-      </c>
-      <c r="E6">
-        <v>164</v>
-      </c>
-      <c r="F6">
-        <v>432</v>
-      </c>
-      <c r="H6">
-        <v>40</v>
-      </c>
-      <c r="I6">
-        <v>780</v>
-      </c>
-      <c r="J6">
-        <v>39</v>
-      </c>
-      <c r="K6">
-        <v>780</v>
-      </c>
-      <c r="L6">
-        <v>780</v>
-      </c>
-      <c r="M6">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="18" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
         <v>50</v>
       </c>
-      <c r="B7">
+      <c r="B18" s="4">
         <v>1225</v>
       </c>
-      <c r="C7">
-        <v>605</v>
-      </c>
-      <c r="D7">
+      <c r="C18" s="4">
+        <v>49</v>
+      </c>
+      <c r="D18" s="4">
         <v>1225</v>
       </c>
-      <c r="E7">
-        <v>228</v>
-      </c>
-      <c r="F7">
-        <v>572</v>
-      </c>
-      <c r="H7">
-        <v>50</v>
-      </c>
-      <c r="I7">
+      <c r="E18" s="4">
         <v>1225</v>
       </c>
-      <c r="J7">
-        <v>49</v>
-      </c>
-      <c r="K7">
-        <v>1225</v>
-      </c>
-      <c r="L7">
-        <v>1225</v>
-      </c>
-      <c r="M7">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>45</v>
-      </c>
-      <c r="C13">
-        <v>9</v>
-      </c>
-      <c r="D13">
-        <v>45</v>
-      </c>
-      <c r="E13">
-        <v>45</v>
-      </c>
-      <c r="F13">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>20</v>
-      </c>
-      <c r="B14">
-        <v>190</v>
-      </c>
-      <c r="C14">
-        <v>19</v>
-      </c>
-      <c r="D14">
-        <v>190</v>
-      </c>
-      <c r="E14">
-        <v>190</v>
-      </c>
-      <c r="F14">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>30</v>
-      </c>
-      <c r="B15">
-        <v>435</v>
-      </c>
-      <c r="C15">
-        <v>29</v>
-      </c>
-      <c r="D15">
-        <v>435</v>
-      </c>
-      <c r="E15">
-        <v>435</v>
-      </c>
-      <c r="F15">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>40</v>
-      </c>
-      <c r="B16">
-        <v>780</v>
-      </c>
-      <c r="C16">
-        <v>39</v>
-      </c>
-      <c r="D16">
-        <v>780</v>
-      </c>
-      <c r="E16">
-        <v>780</v>
-      </c>
-      <c r="F16">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>50</v>
-      </c>
-      <c r="B17">
-        <v>1225</v>
-      </c>
-      <c r="C17">
-        <v>49</v>
-      </c>
-      <c r="D17">
-        <v>1225</v>
-      </c>
-      <c r="E17">
-        <v>1225</v>
-      </c>
-      <c r="F17">
-        <v>572</v>
+      <c r="F18" s="4">
+        <v>235</v>
+      </c>
+      <c r="G18" s="4">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>